<commit_message>
solved not killed problem of Streamer & Trader when nohup in server
</commit_message>
<xml_diff>
--- a/collector/rev_ledger_excel/xrp_bithumb_okcoin.xlsx
+++ b/collector/rev_ledger_excel/xrp_bithumb_okcoin.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jinj/Desktop/Gazeua/arbitrage-bot/collector/rev_ledger_excel/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAA8A016-256C-7944-9596-EDD72D532675}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="820" yWindow="440" windowWidth="27980" windowHeight="17560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="17560" windowWidth="27980" xWindow="820" yWindow="440"/>
   </bookViews>
   <sheets>
-    <sheet name="ledger" sheetId="1" r:id="rId1"/>
+    <sheet name="ledger" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <definedNames/>
+  <calcPr calcId="179021" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="29">
   <si>
     <t>coin_name</t>
   </si>
@@ -98,50 +92,59 @@
   </si>
   <si>
     <t>2018.09.17 15:48:27</t>
+  </si>
+  <si>
+    <t>2018.09.18 16:42:31</t>
+  </si>
+  <si>
+    <t>2018.09.18 23:23:00</t>
+  </si>
+  <si>
+    <t>2018.09.18 22:44:00</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="0.0000000"/>
-    <numFmt numFmtId="165" formatCode="0.0000%"/>
+    <numFmt formatCode="0.0000000" numFmtId="164"/>
+    <numFmt formatCode="0.0000%" numFmtId="165"/>
   </numFmts>
   <fonts count="3">
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="12"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="12"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="12"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
+        <fgColor theme="8" tint="0.7999816888943144"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -205,95 +208,86 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="24">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="2" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="5" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="4" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="2" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="3" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="4" fillId="0" fontId="1" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="4" fillId="0" fontId="1" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="4" fillId="2" fontId="1" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="2" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="0" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="5" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle builtinId="5" name="Percent" xfId="1"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
 </styleSheet>
 </file>
 
@@ -593,38 +587,42 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:R12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="B1:R26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="12" customWidth="1"/>
-    <col min="2" max="2" width="19.5" style="12" customWidth="1"/>
-    <col min="3" max="3" width="14" style="12" customWidth="1"/>
-    <col min="4" max="4" width="15.33203125" style="12" customWidth="1"/>
-    <col min="5" max="5" width="13.1640625" style="12" customWidth="1"/>
-    <col min="6" max="6" width="13" style="12" customWidth="1"/>
-    <col min="7" max="7" width="13.83203125" style="12" customWidth="1"/>
-    <col min="8" max="8" width="13.1640625" style="12" customWidth="1"/>
-    <col min="9" max="9" width="13" style="12" customWidth="1"/>
-    <col min="10" max="10" width="11.5" style="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.5" style="13" customWidth="1"/>
-    <col min="12" max="12" width="13" style="14" customWidth="1"/>
-    <col min="13" max="13" width="13" style="15" customWidth="1"/>
-    <col min="14" max="14" width="12.83203125" style="12" customWidth="1"/>
-    <col min="15" max="24" width="10.83203125" style="12" customWidth="1"/>
-    <col min="25" max="16384" width="10.83203125" style="12"/>
+    <col customWidth="1" max="1" min="1" style="20" width="10.83203125"/>
+    <col customWidth="1" max="2" min="2" style="20" width="19.5"/>
+    <col customWidth="1" max="3" min="3" style="20" width="14"/>
+    <col customWidth="1" max="4" min="4" style="20" width="15.33203125"/>
+    <col customWidth="1" max="5" min="5" style="20" width="13.1640625"/>
+    <col customWidth="1" max="6" min="6" style="20" width="13"/>
+    <col customWidth="1" max="7" min="7" style="20" width="13.83203125"/>
+    <col customWidth="1" max="8" min="8" style="20" width="13.1640625"/>
+    <col customWidth="1" max="9" min="9" style="20" width="13"/>
+    <col bestFit="1" customWidth="1" max="10" min="10" style="20" width="11.5"/>
+    <col customWidth="1" max="11" min="11" style="21" width="11.5"/>
+    <col customWidth="1" max="12" min="12" style="22" width="13"/>
+    <col customWidth="1" max="13" min="13" style="23" width="13"/>
+    <col customWidth="1" max="14" min="14" style="20" width="12.83203125"/>
+    <col customWidth="1" max="24" min="15" style="20" width="10.83203125"/>
+    <col customWidth="1" max="16384" min="25" style="20" width="10.83203125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:18">
-      <c r="D1" s="1"/>
-    </row>
-    <row r="2" spans="2:18">
-      <c r="B2" s="1"/>
+    <row r="1" spans="1:18">
+      <c r="D1" s="1" t="n"/>
+    </row>
+    <row r="2" spans="1:18">
+      <c r="B2" s="1" t="n"/>
       <c r="C2" s="5" t="s">
         <v>0</v>
       </c>
@@ -635,7 +633,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="2:18">
+    <row r="3" spans="1:18">
       <c r="B3" s="5" t="s">
         <v>3</v>
       </c>
@@ -649,57 +647,49 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="2:18">
-      <c r="B4" s="6"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="16"/>
-      <c r="L4" s="17"/>
-      <c r="M4" s="18"/>
-      <c r="O4" s="1"/>
-      <c r="P4" s="1"/>
-      <c r="Q4" s="1"/>
-      <c r="R4" s="1"/>
-    </row>
-    <row r="5" spans="2:18" ht="17" customHeight="1" thickBot="1">
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="19" t="str">
+    <row r="4" spans="1:18">
+      <c r="B4" s="6" t="n"/>
+      <c r="D4" s="2" t="n"/>
+      <c r="E4" s="1" t="n"/>
+      <c r="F4" s="1" t="n"/>
+      <c r="G4" s="1" t="n"/>
+      <c r="H4" s="1" t="n"/>
+      <c r="I4" s="1" t="n"/>
+      <c r="J4" s="1" t="n"/>
+      <c r="K4" s="16" t="n"/>
+      <c r="L4" s="17" t="n"/>
+      <c r="M4" s="18" t="n"/>
+      <c r="O4" s="1" t="n"/>
+      <c r="P4" s="1" t="n"/>
+      <c r="Q4" s="1" t="n"/>
+      <c r="R4" s="1" t="n"/>
+    </row>
+    <row customHeight="1" ht="17" r="5" spans="1:18" thickBot="1">
+      <c r="B5" s="3" t="n"/>
+      <c r="C5" s="3" t="n"/>
+      <c r="D5" s="19">
         <f>UPPER(D3)</f>
-        <v>BITHUMB</v>
-      </c>
-      <c r="E5" s="20"/>
-      <c r="F5" s="19" t="str">
+        <v/>
+      </c>
+      <c r="F5" s="19">
         <f>UPPER(E3)</f>
-        <v>OKCOIN</v>
-      </c>
-      <c r="G5" s="20"/>
+        <v/>
+      </c>
       <c r="H5" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="I5" s="20"/>
       <c r="J5" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="K5" s="21"/>
-      <c r="L5" s="22"/>
-      <c r="M5" s="23"/>
-      <c r="N5" s="7"/>
+      <c r="N5" s="7" t="n"/>
       <c r="O5" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="P5" s="20"/>
       <c r="Q5" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="R5" s="20"/>
-    </row>
-    <row r="6" spans="2:18" ht="17" customHeight="1" thickTop="1">
+    </row>
+    <row customHeight="1" ht="17" r="6" spans="1:18" thickTop="1">
       <c r="B6" s="4" t="s">
         <v>11</v>
       </c>
@@ -709,23 +699,23 @@
       <c r="D6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="4" t="str">
+      <c r="E6" s="4">
         <f>UPPER($C$3)</f>
-        <v>XRP</v>
+        <v/>
       </c>
       <c r="F6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="4" t="str">
+      <c r="G6" s="4">
         <f>UPPER($C$3)</f>
-        <v>XRP</v>
+        <v/>
       </c>
       <c r="H6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="I6" s="4" t="str">
+      <c r="I6" s="4">
         <f>UPPER($C$3)</f>
-        <v>XRP</v>
+        <v/>
       </c>
       <c r="J6" s="4" t="s">
         <v>14</v>
@@ -739,292 +729,656 @@
       <c r="M6" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="N6" s="7"/>
+      <c r="N6" s="7" t="n"/>
       <c r="O6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="P6" s="4" t="str">
+      <c r="P6" s="4">
         <f>UPPER($C$3)</f>
-        <v>XRP</v>
+        <v/>
       </c>
       <c r="Q6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="R6" s="4" t="str">
+      <c r="R6" s="4">
         <f>UPPER($C$3)</f>
-        <v>XRP</v>
-      </c>
-    </row>
-    <row r="7" spans="2:18" ht="17" customHeight="1">
+        <v/>
+      </c>
+    </row>
+    <row customHeight="1" ht="17" r="7" spans="1:18">
       <c r="B7" t="s">
         <v>18</v>
       </c>
       <c r="C7" t="s">
         <v>19</v>
       </c>
-      <c r="D7">
+      <c r="D7" t="n">
         <v>292479</v>
       </c>
-      <c r="E7">
+      <c r="E7" t="n">
         <v>0</v>
       </c>
-      <c r="F7">
-        <v>0.27422999999999997</v>
-      </c>
-      <c r="G7">
-        <v>930.65168000000006</v>
-      </c>
-      <c r="H7">
-        <v>292479.27422999998</v>
-      </c>
-      <c r="I7">
-        <v>930.65168000000006</v>
-      </c>
-      <c r="J7" s="12" t="str">
-        <f t="shared" ref="J7:J12" si="0">IF(C7="settlement", H7-H6, "")</f>
-        <v/>
-      </c>
-      <c r="K7" s="13" t="str">
-        <f t="shared" ref="K7:K12" si="1">IF(C7="settlement", I7-I6,"")</f>
-        <v/>
-      </c>
-      <c r="L7" s="14" t="str">
+      <c r="F7" t="n">
+        <v>0.27423</v>
+      </c>
+      <c r="G7" t="n">
+        <v>930.6516800000001</v>
+      </c>
+      <c r="H7" t="n">
+        <v>292479.27423</v>
+      </c>
+      <c r="I7" t="n">
+        <v>930.6516800000001</v>
+      </c>
+      <c r="J7" s="20">
+        <f>IF(C7="settlement", H7-H6, "")</f>
+        <v/>
+      </c>
+      <c r="K7" s="21">
+        <f>IF(C7="settlement", I7-I6,"")</f>
+        <v/>
+      </c>
+      <c r="L7" s="22">
         <f>IF(C7="settlement", J7/H7, "")</f>
         <v/>
       </c>
-      <c r="M7" s="11" t="str">
+      <c r="M7" s="11">
         <f>IF(C7="settlement", SUM($J$7:J7)/$H$7, "")</f>
         <v/>
       </c>
-      <c r="N7" s="7"/>
-      <c r="O7" s="7"/>
-      <c r="P7" s="7"/>
-      <c r="Q7" s="7"/>
-      <c r="R7" s="7"/>
-    </row>
-    <row r="8" spans="2:18" ht="17" customHeight="1">
+      <c r="N7" s="7" t="n"/>
+      <c r="O7" s="7" t="n"/>
+      <c r="P7" s="7" t="n"/>
+      <c r="Q7" s="7" t="n"/>
+      <c r="R7" s="7" t="n"/>
+    </row>
+    <row customHeight="1" ht="17" r="8" spans="1:18">
       <c r="B8" t="s">
         <v>20</v>
       </c>
       <c r="C8" t="s">
         <v>21</v>
       </c>
-      <c r="D8">
+      <c r="D8" t="n">
         <v>14170</v>
       </c>
-      <c r="E8">
-        <v>929.99788999999998</v>
-      </c>
-      <c r="F8">
-        <v>28074.519230000002</v>
-      </c>
-      <c r="G8">
-        <v>0.65168000000000004</v>
-      </c>
-      <c r="H8">
-        <v>294644.51922999998</v>
-      </c>
-      <c r="I8">
-        <v>930.64957000000004</v>
-      </c>
-      <c r="J8" s="12">
-        <f t="shared" si="0"/>
-        <v>2165.2449999999953</v>
-      </c>
-      <c r="K8" s="13">
-        <f t="shared" si="1"/>
-        <v>-2.1100000000160435E-3</v>
-      </c>
-      <c r="L8" s="14">
+      <c r="E8" t="n">
+        <v>929.99789</v>
+      </c>
+      <c r="F8" t="n">
+        <v>28074.51923</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0.65168</v>
+      </c>
+      <c r="H8" t="n">
+        <v>294644.51923</v>
+      </c>
+      <c r="I8" t="n">
+        <v>930.64957</v>
+      </c>
+      <c r="J8" s="20">
+        <f>IF(C8="settlement", H8-H7, "")</f>
+        <v/>
+      </c>
+      <c r="K8" s="21">
+        <f>IF(C8="settlement", I8-I7,"")</f>
+        <v/>
+      </c>
+      <c r="L8" s="22">
         <f>IF(C8="settlement", J8/H7, "")</f>
-        <v>7.4030715704569514E-3</v>
+        <v/>
       </c>
       <c r="M8" s="11">
         <f>IF(C8="settlement", SUM($J$7:J8)/$H$7, "")</f>
-        <v>7.4030715704569514E-3</v>
-      </c>
-      <c r="N8" s="7"/>
-      <c r="O8" s="7"/>
-      <c r="P8" s="7"/>
-      <c r="Q8" s="7"/>
-      <c r="R8" s="7"/>
-    </row>
-    <row r="9" spans="2:18" ht="17" customHeight="1">
+        <v/>
+      </c>
+      <c r="N8" s="7" t="n"/>
+      <c r="O8" s="7" t="n"/>
+      <c r="P8" s="7" t="n"/>
+      <c r="Q8" s="7" t="n"/>
+      <c r="R8" s="7" t="n"/>
+    </row>
+    <row customHeight="1" ht="17" r="9" spans="1:18">
       <c r="B9" t="s">
         <v>22</v>
       </c>
       <c r="C9" t="s">
         <v>19</v>
       </c>
-      <c r="D9">
+      <c r="D9" t="n">
         <v>280183</v>
       </c>
-      <c r="E9">
-        <v>44.999898000000002</v>
-      </c>
-      <c r="F9">
+      <c r="E9" t="n">
+        <v>44.999898</v>
+      </c>
+      <c r="F9" t="n">
         <v>13487.019226</v>
       </c>
-      <c r="G9">
-        <v>884.64956800000004</v>
-      </c>
-      <c r="H9">
-        <v>293670.01922999998</v>
-      </c>
-      <c r="I9">
-        <v>929.64946999999995</v>
-      </c>
-      <c r="J9" s="12" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="K9" s="13" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="L9" s="14" t="str">
+      <c r="G9" t="n">
+        <v>884.649568</v>
+      </c>
+      <c r="H9" t="n">
+        <v>293670.01923</v>
+      </c>
+      <c r="I9" t="n">
+        <v>929.64947</v>
+      </c>
+      <c r="J9" s="20">
+        <f>IF(C9="settlement", H9-H8, "")</f>
+        <v/>
+      </c>
+      <c r="K9" s="21">
+        <f>IF(C9="settlement", I9-I8,"")</f>
+        <v/>
+      </c>
+      <c r="L9" s="22">
         <f>IF(C9="settlement", J9/H8, "")</f>
         <v/>
       </c>
-      <c r="M9" s="11" t="str">
+      <c r="M9" s="11">
         <f>IF(C9="settlement", SUM($J$7:J9)/$H$7, "")</f>
         <v/>
       </c>
-      <c r="N9" s="7"/>
-      <c r="O9" s="7"/>
-      <c r="P9" s="7"/>
-      <c r="Q9" s="7"/>
-      <c r="R9" s="7"/>
-    </row>
-    <row r="10" spans="2:18" ht="17" customHeight="1">
+      <c r="N9" s="7" t="n"/>
+      <c r="O9" s="7" t="n"/>
+      <c r="P9" s="7" t="n"/>
+      <c r="Q9" s="7" t="n"/>
+      <c r="R9" s="7" t="n"/>
+    </row>
+    <row customHeight="1" ht="17" r="10" spans="1:18">
       <c r="B10" t="s">
         <v>23</v>
       </c>
       <c r="C10" t="s">
         <v>21</v>
       </c>
-      <c r="D10">
+      <c r="D10" t="n">
         <v>270809</v>
       </c>
-      <c r="E10">
-        <v>74.999830000000003</v>
-      </c>
-      <c r="F10">
-        <v>23017.479230000001</v>
-      </c>
-      <c r="G10">
-        <v>854.64957000000004</v>
-      </c>
-      <c r="H10">
+      <c r="E10" t="n">
+        <v>74.99983</v>
+      </c>
+      <c r="F10" t="n">
+        <v>23017.47923</v>
+      </c>
+      <c r="G10" t="n">
+        <v>854.64957</v>
+      </c>
+      <c r="H10" t="n">
         <v>293826.47923</v>
       </c>
-      <c r="I10">
-        <v>929.64940000000001</v>
-      </c>
-      <c r="J10" s="12">
-        <f t="shared" si="0"/>
-        <v>156.46000000002095</v>
-      </c>
-      <c r="K10" s="13">
-        <f t="shared" si="1"/>
-        <v>-6.9999999936953827E-5</v>
-      </c>
-      <c r="L10" s="14">
+      <c r="I10" t="n">
+        <v>929.6494</v>
+      </c>
+      <c r="J10" s="20">
+        <f>IF(C10="settlement", H10-H9, "")</f>
+        <v/>
+      </c>
+      <c r="K10" s="21">
+        <f>IF(C10="settlement", I10-I9,"")</f>
+        <v/>
+      </c>
+      <c r="L10" s="22">
         <f>IF(C10="settlement", J10/H9, "")</f>
-        <v>5.3277484848558124E-4</v>
+        <v/>
       </c>
       <c r="M10" s="11">
         <f>IF(C10="settlement", SUM($J$7:J10)/$H$7, "")</f>
-        <v>7.9380154580603653E-3</v>
-      </c>
-      <c r="N10" s="7"/>
-      <c r="O10" s="7"/>
-      <c r="P10" s="7"/>
-      <c r="Q10" s="7"/>
-      <c r="R10" s="7"/>
-    </row>
-    <row r="11" spans="2:18">
+        <v/>
+      </c>
+      <c r="N10" s="7" t="n"/>
+      <c r="O10" s="7" t="n"/>
+      <c r="P10" s="7" t="n"/>
+      <c r="Q10" s="7" t="n"/>
+      <c r="R10" s="7" t="n"/>
+    </row>
+    <row r="11" spans="1:18">
       <c r="B11" t="s">
         <v>24</v>
       </c>
       <c r="C11" t="s">
         <v>19</v>
       </c>
-      <c r="D11">
+      <c r="D11" t="n">
         <v>270809</v>
       </c>
-      <c r="E11">
-        <v>74.999830000000003</v>
-      </c>
-      <c r="F11">
+      <c r="E11" t="n">
+        <v>74.99983</v>
+      </c>
+      <c r="F11" t="n">
         <v>23017.479225625</v>
       </c>
-      <c r="G11">
-        <v>854.64956832500002</v>
-      </c>
-      <c r="H11">
-        <v>293826.47922562499</v>
-      </c>
-      <c r="I11">
-        <v>929.64939832499999</v>
-      </c>
-      <c r="J11" s="12" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="K11" s="13" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="L11" s="14" t="str">
+      <c r="G11" t="n">
+        <v>854.649568325</v>
+      </c>
+      <c r="H11" t="n">
+        <v>293826.479225625</v>
+      </c>
+      <c r="I11" t="n">
+        <v>929.649398325</v>
+      </c>
+      <c r="J11" s="20">
+        <f>IF(C11="settlement", H11-H10, "")</f>
+        <v/>
+      </c>
+      <c r="K11" s="21">
+        <f>IF(C11="settlement", I11-I10,"")</f>
+        <v/>
+      </c>
+      <c r="L11" s="22">
         <f>IF(C11="settlement", J11/H10, "")</f>
         <v/>
       </c>
-      <c r="M11" s="11" t="str">
+      <c r="M11" s="11">
         <f>IF(C11="settlement", SUM($J$7:J11)/$H$7, "")</f>
         <v/>
       </c>
     </row>
-    <row r="12" spans="2:18">
+    <row r="12" spans="1:18">
       <c r="B12" t="s">
         <v>25</v>
       </c>
       <c r="C12" t="s">
         <v>21</v>
       </c>
-      <c r="D12">
+      <c r="D12" t="n">
         <v>199154</v>
       </c>
-      <c r="E12">
-        <v>299.99932000000001</v>
-      </c>
-      <c r="F12">
-        <v>94720.704225624999</v>
-      </c>
-      <c r="G12">
-        <v>629.64956832500002</v>
-      </c>
-      <c r="H12">
-        <v>293874.70422562503</v>
-      </c>
-      <c r="I12">
-        <v>929.64888832500003</v>
-      </c>
-      <c r="J12" s="12">
-        <f t="shared" si="0"/>
-        <v>48.225000000034925</v>
-      </c>
-      <c r="K12" s="13">
-        <f t="shared" si="1"/>
-        <v>-5.09999999962929E-4</v>
-      </c>
-      <c r="L12" s="14">
+      <c r="E12" t="n">
+        <v>299.99932</v>
+      </c>
+      <c r="F12" t="n">
+        <v>94720.704225625</v>
+      </c>
+      <c r="G12" t="n">
+        <v>629.649568325</v>
+      </c>
+      <c r="H12" t="n">
+        <v>293874.704225625</v>
+      </c>
+      <c r="I12" t="n">
+        <v>929.648888325</v>
+      </c>
+      <c r="J12" s="20">
+        <f>IF(C12="settlement", H12-H11, "")</f>
+        <v/>
+      </c>
+      <c r="K12" s="21">
+        <f>IF(C12="settlement", I12-I11,"")</f>
+        <v/>
+      </c>
+      <c r="L12" s="22">
         <f>IF(C12="settlement", J12/H11, "")</f>
-        <v>1.6412748138673936E-4</v>
+        <v/>
       </c>
       <c r="M12" s="11">
         <f>IF(C12="settlement", SUM($J$7:J12)/$H$7, "")</f>
-        <v>8.1028989361358467E-3</v>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:18">
+      <c r="B13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" t="n">
+        <v>111274</v>
+      </c>
+      <c r="E13" t="n">
+        <v>579.998676</v>
+      </c>
+      <c r="F13" t="n">
+        <v>182992.344225625</v>
+      </c>
+      <c r="G13" t="n">
+        <v>349.649568325</v>
+      </c>
+      <c r="H13" t="n">
+        <v>294266.344225625</v>
+      </c>
+      <c r="I13" t="n">
+        <v>929.6482443250001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18">
+      <c r="B14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" t="n">
+        <v>248070</v>
+      </c>
+      <c r="E14" t="n">
+        <v>159.998676</v>
+      </c>
+      <c r="F14" t="n">
+        <v>47241.729225625</v>
+      </c>
+      <c r="G14" t="n">
+        <v>769.6491483250001</v>
+      </c>
+      <c r="H14" t="n">
+        <v>295311.729225625</v>
+      </c>
+      <c r="I14" t="n">
+        <v>929.6478243250001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18">
+      <c r="B15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" t="n">
+        <v>248070</v>
+      </c>
+      <c r="E15" t="n">
+        <v>159.998676</v>
+      </c>
+      <c r="F15" t="n">
+        <v>47241.729225625</v>
+      </c>
+      <c r="G15" t="n">
+        <v>769.6491483250001</v>
+      </c>
+      <c r="H15" t="n">
+        <v>295311.729225625</v>
+      </c>
+      <c r="I15" t="n">
+        <v>929.6478243250001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18">
+      <c r="B16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" t="n">
+        <v>248070</v>
+      </c>
+      <c r="E16" t="n">
+        <v>159.998676</v>
+      </c>
+      <c r="F16" t="n">
+        <v>47241.729225625</v>
+      </c>
+      <c r="G16" t="n">
+        <v>769.6491483250001</v>
+      </c>
+      <c r="H16" t="n">
+        <v>295311.729225625</v>
+      </c>
+      <c r="I16" t="n">
+        <v>929.6478243250001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18">
+      <c r="B17" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" t="n">
+        <v>248070</v>
+      </c>
+      <c r="E17" t="n">
+        <v>159.998676</v>
+      </c>
+      <c r="F17" t="n">
+        <v>47241.729225625</v>
+      </c>
+      <c r="G17" t="n">
+        <v>769.6491483250001</v>
+      </c>
+      <c r="H17" t="n">
+        <v>295311.729225625</v>
+      </c>
+      <c r="I17" t="n">
+        <v>929.6478243250001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18">
+      <c r="B18" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" t="n">
+        <v>248070</v>
+      </c>
+      <c r="E18" t="n">
+        <v>159.998676</v>
+      </c>
+      <c r="F18" t="n">
+        <v>47241.729225625</v>
+      </c>
+      <c r="G18" t="n">
+        <v>769.6491483250001</v>
+      </c>
+      <c r="H18" t="n">
+        <v>295311.729225625</v>
+      </c>
+      <c r="I18" t="n">
+        <v>929.6478243250001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18">
+      <c r="B19" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" t="s">
+        <v>19</v>
+      </c>
+      <c r="D19" t="n">
+        <v>248070</v>
+      </c>
+      <c r="E19" t="n">
+        <v>159.998676</v>
+      </c>
+      <c r="F19" t="n">
+        <v>47241.729225625</v>
+      </c>
+      <c r="G19" t="n">
+        <v>769.6491483250001</v>
+      </c>
+      <c r="H19" t="n">
+        <v>295311.729225625</v>
+      </c>
+      <c r="I19" t="n">
+        <v>929.6478243250001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18">
+      <c r="B20" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" t="s">
+        <v>21</v>
+      </c>
+      <c r="D20" t="n">
+        <v>248070</v>
+      </c>
+      <c r="E20" t="n">
+        <v>159.998676</v>
+      </c>
+      <c r="F20" t="n">
+        <v>47241.729225625</v>
+      </c>
+      <c r="G20" t="n">
+        <v>769.6491483250001</v>
+      </c>
+      <c r="H20" t="n">
+        <v>295311.729225625</v>
+      </c>
+      <c r="I20" t="n">
+        <v>929.6478243250001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18">
+      <c r="B21" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21" t="n">
+        <v>248070</v>
+      </c>
+      <c r="E21" t="n">
+        <v>159.998676</v>
+      </c>
+      <c r="F21" t="n">
+        <v>47241.729225625</v>
+      </c>
+      <c r="G21" t="n">
+        <v>769.6491483250001</v>
+      </c>
+      <c r="H21" t="n">
+        <v>295311.729225625</v>
+      </c>
+      <c r="I21" t="n">
+        <v>929.6478243250001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18">
+      <c r="B22" t="s">
+        <v>28</v>
+      </c>
+      <c r="C22" t="s">
+        <v>21</v>
+      </c>
+      <c r="D22" t="n">
+        <v>248070</v>
+      </c>
+      <c r="E22" t="n">
+        <v>159.998676</v>
+      </c>
+      <c r="F22" t="n">
+        <v>47241.729225625</v>
+      </c>
+      <c r="G22" t="n">
+        <v>769.6491483250001</v>
+      </c>
+      <c r="H22" t="n">
+        <v>295311.729225625</v>
+      </c>
+      <c r="I22" t="n">
+        <v>929.6478243250001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18">
+      <c r="B23" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23" t="s">
+        <v>19</v>
+      </c>
+      <c r="D23" t="n">
+        <v>248070</v>
+      </c>
+      <c r="E23" t="n">
+        <v>159.998676</v>
+      </c>
+      <c r="F23" t="n">
+        <v>47241.729225625</v>
+      </c>
+      <c r="G23" t="n">
+        <v>769.6491483250001</v>
+      </c>
+      <c r="H23" t="n">
+        <v>295311.729225625</v>
+      </c>
+      <c r="I23" t="n">
+        <v>929.6478243250001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18">
+      <c r="B24" t="s">
+        <v>28</v>
+      </c>
+      <c r="C24" t="s">
+        <v>21</v>
+      </c>
+      <c r="D24" t="n">
+        <v>248070</v>
+      </c>
+      <c r="E24" t="n">
+        <v>159.998676</v>
+      </c>
+      <c r="F24" t="n">
+        <v>47241.729225625</v>
+      </c>
+      <c r="G24" t="n">
+        <v>769.6491483250001</v>
+      </c>
+      <c r="H24" t="n">
+        <v>295311.729225625</v>
+      </c>
+      <c r="I24" t="n">
+        <v>929.6478243250001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18">
+      <c r="B25" t="s">
+        <v>27</v>
+      </c>
+      <c r="C25" t="s">
+        <v>19</v>
+      </c>
+      <c r="D25" t="n">
+        <v>248070</v>
+      </c>
+      <c r="E25" t="n">
+        <v>159.998676</v>
+      </c>
+      <c r="F25" t="n">
+        <v>47241.729225625</v>
+      </c>
+      <c r="G25" t="n">
+        <v>769.6491483250001</v>
+      </c>
+      <c r="H25" t="n">
+        <v>295311.729225625</v>
+      </c>
+      <c r="I25" t="n">
+        <v>929.6478243250001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18">
+      <c r="B26" t="s">
+        <v>28</v>
+      </c>
+      <c r="C26" t="s">
+        <v>21</v>
+      </c>
+      <c r="D26" t="n">
+        <v>248070</v>
+      </c>
+      <c r="E26" t="n">
+        <v>159.998676</v>
+      </c>
+      <c r="F26" t="n">
+        <v>47241.729225625</v>
+      </c>
+      <c r="G26" t="n">
+        <v>769.6491483250001</v>
+      </c>
+      <c r="H26" t="n">
+        <v>295311.729225625</v>
+      </c>
+      <c r="I26" t="n">
+        <v>929.6478243250001</v>
       </c>
     </row>
   </sheetData>
@@ -1036,7 +1390,7 @@
     <mergeCell ref="H5:I5"/>
     <mergeCell ref="J5:M5"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
grand refactoring done for Streamer and Handler.. Now can conduct NEW, REV at the same time
</commit_message>
<xml_diff>
--- a/collector/rev_ledger_excel/xrp_bithumb_okcoin.xlsx
+++ b/collector/rev_ledger_excel/xrp_bithumb_okcoin.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="40">
   <si>
     <t>coin_name</t>
   </si>
@@ -128,6 +128,12 @@
   </si>
   <si>
     <t>2018.09.20 10:12:33</t>
+  </si>
+  <si>
+    <t>2018.09.21 16:03:50</t>
+  </si>
+  <si>
+    <t>2018.09.21 20:19:14</t>
   </si>
 </sst>
 </file>
@@ -654,7 +660,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B1:R26"/>
+  <dimension ref="B1:R31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="M2" sqref="M2"/>
@@ -727,7 +733,7 @@
         <v>7</v>
       </c>
       <c r="C5" s="29">
-        <f>SUM(J11:J26)</f>
+        <f>SUM(J11:J31)</f>
         <v/>
       </c>
       <c r="D5" s="29" t="n"/>
@@ -742,7 +748,7 @@
         <v>8</v>
       </c>
       <c r="C6" s="30">
-        <f>SUM(K11:K26)</f>
+        <f>SUM(K11:K31)</f>
         <v/>
       </c>
       <c r="D6" s="29" t="n"/>
@@ -757,7 +763,7 @@
         <v>9</v>
       </c>
       <c r="C7" s="16">
-        <f>M26</f>
+        <f>M31</f>
         <v/>
       </c>
       <c r="D7" s="29" t="n"/>
@@ -1538,6 +1544,216 @@
         <v/>
       </c>
     </row>
+    <row r="27" spans="1:18">
+      <c r="B27" t="s">
+        <v>38</v>
+      </c>
+      <c r="C27" t="s">
+        <v>21</v>
+      </c>
+      <c r="D27" t="n">
+        <v>184903</v>
+      </c>
+      <c r="E27" t="n">
+        <v>324.999336</v>
+      </c>
+      <c r="F27" t="n">
+        <v>237558.573525625</v>
+      </c>
+      <c r="G27" t="n">
+        <v>357.444562325</v>
+      </c>
+      <c r="H27" t="n">
+        <v>422461.573525625</v>
+      </c>
+      <c r="I27" t="n">
+        <v>682.443898325</v>
+      </c>
+      <c r="J27">
+        <f>IF(C27="settlement", H27-H26, "")</f>
+        <v/>
+      </c>
+      <c r="K27">
+        <f>IF(C27="settlement", I27-I26, "")</f>
+        <v/>
+      </c>
+      <c r="L27" s="34">
+        <f>IF(C27="settlement", J27/H26, "")</f>
+        <v/>
+      </c>
+      <c r="M27" s="35">
+        <f>IF(C27="settlement", SUM($J$11:J27)/$H$11, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="28" spans="1:18">
+      <c r="B28" t="s">
+        <v>38</v>
+      </c>
+      <c r="C28" t="s">
+        <v>21</v>
+      </c>
+      <c r="D28" t="n">
+        <v>184903</v>
+      </c>
+      <c r="E28" t="n">
+        <v>324.999336</v>
+      </c>
+      <c r="F28" t="n">
+        <v>237558.573525625</v>
+      </c>
+      <c r="G28" t="n">
+        <v>357.444562325</v>
+      </c>
+      <c r="H28" t="n">
+        <v>422461.573525625</v>
+      </c>
+      <c r="I28" t="n">
+        <v>682.443898325</v>
+      </c>
+      <c r="J28">
+        <f>IF(C28="settlement", H28-H27, "")</f>
+        <v/>
+      </c>
+      <c r="K28">
+        <f>IF(C28="settlement", I28-I27, "")</f>
+        <v/>
+      </c>
+      <c r="L28" s="34">
+        <f>IF(C28="settlement", J28/H27, "")</f>
+        <v/>
+      </c>
+      <c r="M28" s="35">
+        <f>IF(C28="settlement", SUM($J$11:J28)/$H$11, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="29" spans="1:18">
+      <c r="B29" t="s">
+        <v>38</v>
+      </c>
+      <c r="C29" t="s">
+        <v>21</v>
+      </c>
+      <c r="D29" t="n">
+        <v>184903</v>
+      </c>
+      <c r="E29" t="n">
+        <v>324.999336</v>
+      </c>
+      <c r="F29" t="n">
+        <v>237558.573525625</v>
+      </c>
+      <c r="G29" t="n">
+        <v>357.444562325</v>
+      </c>
+      <c r="H29" t="n">
+        <v>422461.573525625</v>
+      </c>
+      <c r="I29" t="n">
+        <v>682.443898325</v>
+      </c>
+      <c r="J29">
+        <f>IF(C29="settlement", H29-H28, "")</f>
+        <v/>
+      </c>
+      <c r="K29">
+        <f>IF(C29="settlement", I29-I28, "")</f>
+        <v/>
+      </c>
+      <c r="L29" s="34">
+        <f>IF(C29="settlement", J29/H28, "")</f>
+        <v/>
+      </c>
+      <c r="M29" s="35">
+        <f>IF(C29="settlement", SUM($J$11:J29)/$H$11, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="30" spans="1:18">
+      <c r="B30" t="s">
+        <v>38</v>
+      </c>
+      <c r="C30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D30" t="n">
+        <v>184903</v>
+      </c>
+      <c r="E30" t="n">
+        <v>324.999336</v>
+      </c>
+      <c r="F30" t="n">
+        <v>237558.573525625</v>
+      </c>
+      <c r="G30" t="n">
+        <v>357.444562325</v>
+      </c>
+      <c r="H30" t="n">
+        <v>422461.573525625</v>
+      </c>
+      <c r="I30" t="n">
+        <v>682.443898325</v>
+      </c>
+      <c r="J30">
+        <f>IF(C30="settlement", H30-H29, "")</f>
+        <v/>
+      </c>
+      <c r="K30">
+        <f>IF(C30="settlement", I30-I29, "")</f>
+        <v/>
+      </c>
+      <c r="L30" s="34">
+        <f>IF(C30="settlement", J30/H29, "")</f>
+        <v/>
+      </c>
+      <c r="M30" s="35">
+        <f>IF(C30="settlement", SUM($J$11:J30)/$H$11, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="31" spans="1:18">
+      <c r="B31" t="s">
+        <v>39</v>
+      </c>
+      <c r="C31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D31" t="n">
+        <v>213883</v>
+      </c>
+      <c r="E31" t="n">
+        <v>368.999236</v>
+      </c>
+      <c r="F31" t="n">
+        <v>374333.661525625</v>
+      </c>
+      <c r="G31" t="n">
+        <v>355.991847325</v>
+      </c>
+      <c r="H31" t="n">
+        <v>588216.661525625</v>
+      </c>
+      <c r="I31" t="n">
+        <v>724.991083325</v>
+      </c>
+      <c r="J31">
+        <f>IF(C31="settlement", H31-H30, "")</f>
+        <v/>
+      </c>
+      <c r="K31">
+        <f>IF(C31="settlement", I31-I30, "")</f>
+        <v/>
+      </c>
+      <c r="L31" s="34">
+        <f>IF(C31="settlement", J31/H30, "")</f>
+        <v/>
+      </c>
+      <c r="M31" s="35">
+        <f>IF(C31="settlement", SUM($J$11:J31)/$H$11, "")</f>
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="O9:P9"/>

</xml_diff>

<commit_message>
refactoring for Streamer & Trader Done
</commit_message>
<xml_diff>
--- a/collector/rev_ledger_excel/xrp_bithumb_okcoin.xlsx
+++ b/collector/rev_ledger_excel/xrp_bithumb_okcoin.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="50">
   <si>
     <t>coin_name</t>
   </si>
@@ -134,6 +134,36 @@
   </si>
   <si>
     <t>2018.09.21 20:19:14</t>
+  </si>
+  <si>
+    <t>2018.09.22 00:37:06</t>
+  </si>
+  <si>
+    <t>2018.09.22 00:48:20</t>
+  </si>
+  <si>
+    <t>2018.09.22 00:55:02</t>
+  </si>
+  <si>
+    <t>2018.09.22 01:58:35</t>
+  </si>
+  <si>
+    <t>2018.09.22 01:59:37</t>
+  </si>
+  <si>
+    <t>2018.09.22 02:02:25</t>
+  </si>
+  <si>
+    <t>2018.09.22 02:03:49</t>
+  </si>
+  <si>
+    <t>2018.09.22 02:04:51</t>
+  </si>
+  <si>
+    <t>2018.09.22 02:11:10</t>
+  </si>
+  <si>
+    <t>2018.09.22 02:12:18</t>
   </si>
 </sst>
 </file>
@@ -660,7 +690,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B1:R31"/>
+  <dimension ref="B1:R43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="M2" sqref="M2"/>
@@ -733,7 +763,7 @@
         <v>7</v>
       </c>
       <c r="C5" s="29">
-        <f>SUM(J11:J31)</f>
+        <f>SUM(J11:J43)</f>
         <v/>
       </c>
       <c r="D5" s="29" t="n"/>
@@ -748,7 +778,7 @@
         <v>8</v>
       </c>
       <c r="C6" s="30">
-        <f>SUM(K11:K31)</f>
+        <f>SUM(K11:K43)</f>
         <v/>
       </c>
       <c r="D6" s="29" t="n"/>
@@ -763,7 +793,7 @@
         <v>9</v>
       </c>
       <c r="C7" s="16">
-        <f>M31</f>
+        <f>M43</f>
         <v/>
       </c>
       <c r="D7" s="29" t="n"/>
@@ -1754,6 +1784,510 @@
         <v/>
       </c>
     </row>
+    <row r="32" spans="1:18">
+      <c r="B32" t="s">
+        <v>39</v>
+      </c>
+      <c r="C32" t="s">
+        <v>21</v>
+      </c>
+      <c r="D32" t="n">
+        <v>213883</v>
+      </c>
+      <c r="E32" t="n">
+        <v>368.999236</v>
+      </c>
+      <c r="F32" t="n">
+        <v>374333.661525625</v>
+      </c>
+      <c r="G32" t="n">
+        <v>355.991847325</v>
+      </c>
+      <c r="H32" t="n">
+        <v>588216.661525625</v>
+      </c>
+      <c r="I32" t="n">
+        <v>724.991083325</v>
+      </c>
+      <c r="J32">
+        <f>IF(C32="settlement", H32-H31, "")</f>
+        <v/>
+      </c>
+      <c r="K32">
+        <f>IF(C32="settlement", I32-I31, "")</f>
+        <v/>
+      </c>
+      <c r="L32" s="34">
+        <f>IF(C32="settlement", J32/H31, "")</f>
+        <v/>
+      </c>
+      <c r="M32" s="35">
+        <f>IF(C32="settlement", SUM($J$11:J32)/$H$11, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="33" spans="1:18">
+      <c r="B33" t="s">
+        <v>39</v>
+      </c>
+      <c r="C33" t="s">
+        <v>21</v>
+      </c>
+      <c r="D33" t="n">
+        <v>213883</v>
+      </c>
+      <c r="E33" t="n">
+        <v>368.999236</v>
+      </c>
+      <c r="F33" t="n">
+        <v>374333.661525625</v>
+      </c>
+      <c r="G33" t="n">
+        <v>355.991847325</v>
+      </c>
+      <c r="H33" t="n">
+        <v>588216.661525625</v>
+      </c>
+      <c r="I33" t="n">
+        <v>724.991083325</v>
+      </c>
+      <c r="J33">
+        <f>IF(C33="settlement", H33-H32, "")</f>
+        <v/>
+      </c>
+      <c r="K33">
+        <f>IF(C33="settlement", I33-I32, "")</f>
+        <v/>
+      </c>
+      <c r="L33" s="34">
+        <f>IF(C33="settlement", J33/H32, "")</f>
+        <v/>
+      </c>
+      <c r="M33" s="35">
+        <f>IF(C33="settlement", SUM($J$11:J33)/$H$11, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="34" spans="1:18">
+      <c r="B34" t="s">
+        <v>40</v>
+      </c>
+      <c r="C34" t="s">
+        <v>21</v>
+      </c>
+      <c r="D34" t="n">
+        <v>344379</v>
+      </c>
+      <c r="E34" t="n">
+        <v>152.999236</v>
+      </c>
+      <c r="F34" t="n">
+        <v>251829.180347625</v>
+      </c>
+      <c r="G34" t="n">
+        <v>571.991631325</v>
+      </c>
+      <c r="H34" t="n">
+        <v>596208.1803476249</v>
+      </c>
+      <c r="I34" t="n">
+        <v>724.990867325</v>
+      </c>
+      <c r="J34">
+        <f>IF(C34="settlement", H34-H33, "")</f>
+        <v/>
+      </c>
+      <c r="K34">
+        <f>IF(C34="settlement", I34-I33, "")</f>
+        <v/>
+      </c>
+      <c r="L34" s="34">
+        <f>IF(C34="settlement", J34/H33, "")</f>
+        <v/>
+      </c>
+      <c r="M34" s="35">
+        <f>IF(C34="settlement", SUM($J$11:J34)/$H$11, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="35" spans="1:18">
+      <c r="B35" t="s">
+        <v>41</v>
+      </c>
+      <c r="C35" t="s">
+        <v>21</v>
+      </c>
+      <c r="D35" t="n">
+        <v>344379</v>
+      </c>
+      <c r="E35" t="n">
+        <v>152.999236</v>
+      </c>
+      <c r="F35" t="n">
+        <v>251829.180347625</v>
+      </c>
+      <c r="G35" t="n">
+        <v>571.991631325</v>
+      </c>
+      <c r="H35" t="n">
+        <v>596208.1803476249</v>
+      </c>
+      <c r="I35" t="n">
+        <v>724.990867325</v>
+      </c>
+      <c r="J35">
+        <f>IF(C35="settlement", H35-H34, "")</f>
+        <v/>
+      </c>
+      <c r="K35">
+        <f>IF(C35="settlement", I35-I34, "")</f>
+        <v/>
+      </c>
+      <c r="L35" s="34">
+        <f>IF(C35="settlement", J35/H34, "")</f>
+        <v/>
+      </c>
+      <c r="M35" s="35">
+        <f>IF(C35="settlement", SUM($J$11:J35)/$H$11, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="36" spans="1:18">
+      <c r="B36" t="s">
+        <v>42</v>
+      </c>
+      <c r="C36" t="s">
+        <v>21</v>
+      </c>
+      <c r="D36" t="n">
+        <v>344379</v>
+      </c>
+      <c r="E36" t="n">
+        <v>152.999236</v>
+      </c>
+      <c r="F36" t="n">
+        <v>251829.180347625</v>
+      </c>
+      <c r="G36" t="n">
+        <v>571.991631325</v>
+      </c>
+      <c r="H36" t="n">
+        <v>596208.1803476249</v>
+      </c>
+      <c r="I36" t="n">
+        <v>724.990867325</v>
+      </c>
+      <c r="J36">
+        <f>IF(C36="settlement", H36-H35, "")</f>
+        <v/>
+      </c>
+      <c r="K36">
+        <f>IF(C36="settlement", I36-I35, "")</f>
+        <v/>
+      </c>
+      <c r="L36" s="34">
+        <f>IF(C36="settlement", J36/H35, "")</f>
+        <v/>
+      </c>
+      <c r="M36" s="35">
+        <f>IF(C36="settlement", SUM($J$11:J36)/$H$11, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="37" spans="1:18">
+      <c r="B37" t="s">
+        <v>43</v>
+      </c>
+      <c r="C37" t="s">
+        <v>21</v>
+      </c>
+      <c r="D37" t="n">
+        <v>344379</v>
+      </c>
+      <c r="E37" t="n">
+        <v>152.999236</v>
+      </c>
+      <c r="F37" t="n">
+        <v>251829.180347625</v>
+      </c>
+      <c r="G37" t="n">
+        <v>571.991631325</v>
+      </c>
+      <c r="H37" t="n">
+        <v>596208.1803476249</v>
+      </c>
+      <c r="I37" t="n">
+        <v>724.990867325</v>
+      </c>
+      <c r="J37">
+        <f>IF(C37="settlement", H37-H36, "")</f>
+        <v/>
+      </c>
+      <c r="K37">
+        <f>IF(C37="settlement", I37-I36, "")</f>
+        <v/>
+      </c>
+      <c r="L37" s="34">
+        <f>IF(C37="settlement", J37/H36, "")</f>
+        <v/>
+      </c>
+      <c r="M37" s="35">
+        <f>IF(C37="settlement", SUM($J$11:J37)/$H$11, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="38" spans="1:18">
+      <c r="B38" t="s">
+        <v>44</v>
+      </c>
+      <c r="C38" t="s">
+        <v>21</v>
+      </c>
+      <c r="D38" t="n">
+        <v>344379</v>
+      </c>
+      <c r="E38" t="n">
+        <v>152.999236</v>
+      </c>
+      <c r="F38" t="n">
+        <v>251829.180347625</v>
+      </c>
+      <c r="G38" t="n">
+        <v>571.991631325</v>
+      </c>
+      <c r="H38" t="n">
+        <v>596208.1803476249</v>
+      </c>
+      <c r="I38" t="n">
+        <v>724.990867325</v>
+      </c>
+      <c r="J38">
+        <f>IF(C38="settlement", H38-H37, "")</f>
+        <v/>
+      </c>
+      <c r="K38">
+        <f>IF(C38="settlement", I38-I37, "")</f>
+        <v/>
+      </c>
+      <c r="L38" s="34">
+        <f>IF(C38="settlement", J38/H37, "")</f>
+        <v/>
+      </c>
+      <c r="M38" s="35">
+        <f>IF(C38="settlement", SUM($J$11:J38)/$H$11, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="39" spans="1:18">
+      <c r="B39" t="s">
+        <v>45</v>
+      </c>
+      <c r="C39" t="s">
+        <v>21</v>
+      </c>
+      <c r="D39" t="n">
+        <v>344379</v>
+      </c>
+      <c r="E39" t="n">
+        <v>152.999236</v>
+      </c>
+      <c r="F39" t="n">
+        <v>251829.180347625</v>
+      </c>
+      <c r="G39" t="n">
+        <v>571.991631325</v>
+      </c>
+      <c r="H39" t="n">
+        <v>596208.1803476249</v>
+      </c>
+      <c r="I39" t="n">
+        <v>724.990867325</v>
+      </c>
+      <c r="J39">
+        <f>IF(C39="settlement", H39-H38, "")</f>
+        <v/>
+      </c>
+      <c r="K39">
+        <f>IF(C39="settlement", I39-I38, "")</f>
+        <v/>
+      </c>
+      <c r="L39" s="34">
+        <f>IF(C39="settlement", J39/H38, "")</f>
+        <v/>
+      </c>
+      <c r="M39" s="35">
+        <f>IF(C39="settlement", SUM($J$11:J39)/$H$11, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="40" spans="1:18">
+      <c r="B40" t="s">
+        <v>46</v>
+      </c>
+      <c r="C40" t="s">
+        <v>21</v>
+      </c>
+      <c r="D40" t="n">
+        <v>344379</v>
+      </c>
+      <c r="E40" t="n">
+        <v>152.999236</v>
+      </c>
+      <c r="F40" t="n">
+        <v>251829.180347625</v>
+      </c>
+      <c r="G40" t="n">
+        <v>571.991631325</v>
+      </c>
+      <c r="H40" t="n">
+        <v>596208.1803476249</v>
+      </c>
+      <c r="I40" t="n">
+        <v>724.990867325</v>
+      </c>
+      <c r="J40">
+        <f>IF(C40="settlement", H40-H39, "")</f>
+        <v/>
+      </c>
+      <c r="K40">
+        <f>IF(C40="settlement", I40-I39, "")</f>
+        <v/>
+      </c>
+      <c r="L40" s="34">
+        <f>IF(C40="settlement", J40/H39, "")</f>
+        <v/>
+      </c>
+      <c r="M40" s="35">
+        <f>IF(C40="settlement", SUM($J$11:J40)/$H$11, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="41" spans="1:18">
+      <c r="B41" t="s">
+        <v>47</v>
+      </c>
+      <c r="C41" t="s">
+        <v>21</v>
+      </c>
+      <c r="D41" t="n">
+        <v>344379</v>
+      </c>
+      <c r="E41" t="n">
+        <v>152.999236</v>
+      </c>
+      <c r="F41" t="n">
+        <v>251829.180347625</v>
+      </c>
+      <c r="G41" t="n">
+        <v>571.991631325</v>
+      </c>
+      <c r="H41" t="n">
+        <v>596208.1803476249</v>
+      </c>
+      <c r="I41" t="n">
+        <v>724.990867325</v>
+      </c>
+      <c r="J41">
+        <f>IF(C41="settlement", H41-H40, "")</f>
+        <v/>
+      </c>
+      <c r="K41">
+        <f>IF(C41="settlement", I41-I40, "")</f>
+        <v/>
+      </c>
+      <c r="L41" s="34">
+        <f>IF(C41="settlement", J41/H40, "")</f>
+        <v/>
+      </c>
+      <c r="M41" s="35">
+        <f>IF(C41="settlement", SUM($J$11:J41)/$H$11, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="42" spans="1:18">
+      <c r="B42" t="s">
+        <v>48</v>
+      </c>
+      <c r="C42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D42" t="n">
+        <v>344379</v>
+      </c>
+      <c r="E42" t="n">
+        <v>152.999236</v>
+      </c>
+      <c r="F42" t="n">
+        <v>251829.180347625</v>
+      </c>
+      <c r="G42" t="n">
+        <v>571.991631325</v>
+      </c>
+      <c r="H42" t="n">
+        <v>596208.1803476249</v>
+      </c>
+      <c r="I42" t="n">
+        <v>724.990867325</v>
+      </c>
+      <c r="J42">
+        <f>IF(C42="settlement", H42-H41, "")</f>
+        <v/>
+      </c>
+      <c r="K42">
+        <f>IF(C42="settlement", I42-I41, "")</f>
+        <v/>
+      </c>
+      <c r="L42" s="34">
+        <f>IF(C42="settlement", J42/H41, "")</f>
+        <v/>
+      </c>
+      <c r="M42" s="35">
+        <f>IF(C42="settlement", SUM($J$11:J42)/$H$11, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="43" spans="1:18">
+      <c r="B43" t="s">
+        <v>49</v>
+      </c>
+      <c r="C43" t="s">
+        <v>21</v>
+      </c>
+      <c r="D43" t="n">
+        <v>344379</v>
+      </c>
+      <c r="E43" t="n">
+        <v>152.999236</v>
+      </c>
+      <c r="F43" t="n">
+        <v>251829.180347625</v>
+      </c>
+      <c r="G43" t="n">
+        <v>571.991631325</v>
+      </c>
+      <c r="H43" t="n">
+        <v>596208.1803476249</v>
+      </c>
+      <c r="I43" t="n">
+        <v>724.990867325</v>
+      </c>
+      <c r="J43">
+        <f>IF(C43="settlement", H43-H42, "")</f>
+        <v/>
+      </c>
+      <c r="K43">
+        <f>IF(C43="settlement", I43-I42, "")</f>
+        <v/>
+      </c>
+      <c r="L43" s="34">
+        <f>IF(C43="settlement", J43/H42, "")</f>
+        <v/>
+      </c>
+      <c r="M43" s="35">
+        <f>IF(C43="settlement", SUM($J$11:J43)/$H$11, "")</f>
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="O9:P9"/>

</xml_diff>

<commit_message>
minor error fixed in Handler
</commit_message>
<xml_diff>
--- a/collector/rev_ledger_excel/xrp_bithumb_okcoin.xlsx
+++ b/collector/rev_ledger_excel/xrp_bithumb_okcoin.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="51">
   <si>
     <t>coin_name</t>
   </si>
@@ -164,6 +164,9 @@
   </si>
   <si>
     <t>2018.09.22 02:12:18</t>
+  </si>
+  <si>
+    <t>2018.09.22 02:38:53</t>
   </si>
 </sst>
 </file>
@@ -690,7 +693,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B1:R43"/>
+  <dimension ref="B1:R44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="M2" sqref="M2"/>
@@ -763,7 +766,7 @@
         <v>7</v>
       </c>
       <c r="C5" s="29">
-        <f>SUM(J11:J43)</f>
+        <f>SUM(J11:J44)</f>
         <v/>
       </c>
       <c r="D5" s="29" t="n"/>
@@ -778,7 +781,7 @@
         <v>8</v>
       </c>
       <c r="C6" s="30">
-        <f>SUM(K11:K43)</f>
+        <f>SUM(K11:K44)</f>
         <v/>
       </c>
       <c r="D6" s="29" t="n"/>
@@ -793,7 +796,7 @@
         <v>9</v>
       </c>
       <c r="C7" s="16">
-        <f>M43</f>
+        <f>M44</f>
         <v/>
       </c>
       <c r="D7" s="29" t="n"/>
@@ -2288,6 +2291,48 @@
         <v/>
       </c>
     </row>
+    <row r="44" spans="1:18">
+      <c r="B44" t="s">
+        <v>50</v>
+      </c>
+      <c r="C44" t="s">
+        <v>21</v>
+      </c>
+      <c r="D44" t="n">
+        <v>344379</v>
+      </c>
+      <c r="E44" t="n">
+        <v>152.999236</v>
+      </c>
+      <c r="F44" t="n">
+        <v>251829.180347625</v>
+      </c>
+      <c r="G44" t="n">
+        <v>571.991631325</v>
+      </c>
+      <c r="H44" t="n">
+        <v>596208.1803476249</v>
+      </c>
+      <c r="I44" t="n">
+        <v>724.990867325</v>
+      </c>
+      <c r="J44">
+        <f>IF(C44="settlement", H44-H43, "")</f>
+        <v/>
+      </c>
+      <c r="K44">
+        <f>IF(C44="settlement", I44-I43, "")</f>
+        <v/>
+      </c>
+      <c r="L44" s="34">
+        <f>IF(C44="settlement", J44/H43, "")</f>
+        <v/>
+      </c>
+      <c r="M44" s="35">
+        <f>IF(C44="settlement", SUM($J$11:J44)/$H$11, "")</f>
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="O9:P9"/>

</xml_diff>